<commit_message>
Adding parameters for IDU time until regular injector
</commit_message>
<xml_diff>
--- a/data/excelsheets/timeuntilregularinjector.xlsx
+++ b/data/excelsheets/timeuntilregularinjector.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="18">
   <si>
     <t>http://www.ncbi.nlm.nih.gov/pmc/articles/PMC3874445/</t>
   </si>
@@ -64,6 +64,12 @@
   </si>
   <si>
     <t>Use a probability to determine time until regular injection</t>
+  </si>
+  <si>
+    <t>Survival</t>
+  </si>
+  <si>
+    <t>Probability</t>
   </si>
 </sst>
 </file>
@@ -402,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:L20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,9 +542,38 @@
         <v>0.36809815950920244</v>
       </c>
     </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" t="s">
+        <v>16</v>
+      </c>
+    </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>11</v>
+      </c>
+      <c r="B13" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" t="s">
+        <v>8</v>
+      </c>
+      <c r="F13" t="s">
+        <v>9</v>
+      </c>
+      <c r="G13" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -558,8 +593,17 @@
         <f t="shared" si="0"/>
         <v>0.5145631067961165</v>
       </c>
-      <c r="F14" t="s">
-        <v>15</v>
+      <c r="E14">
+        <f>1-B14</f>
+        <v>0.54761904761904767</v>
+      </c>
+      <c r="F14">
+        <f>1-C14</f>
+        <v>0.59060402684563762</v>
+      </c>
+      <c r="G14">
+        <f>1-D14</f>
+        <v>0.4854368932038835</v>
       </c>
       <c r="J14" t="s">
         <v>12</v>
@@ -588,6 +632,18 @@
         <f t="shared" si="2"/>
         <v>0.32038834951456313</v>
       </c>
+      <c r="E15">
+        <f>E14-B15</f>
+        <v>0.21031746031746035</v>
+      </c>
+      <c r="F15">
+        <f>F14-C15</f>
+        <v>0.2416107382550336</v>
+      </c>
+      <c r="G15">
+        <f>G14-D15</f>
+        <v>0.16504854368932037</v>
+      </c>
       <c r="J15">
         <f>B14</f>
         <v>0.45238095238095238</v>
@@ -618,6 +674,18 @@
         <f t="shared" si="2"/>
         <v>3.8834951456310676E-2</v>
       </c>
+      <c r="E16">
+        <f t="shared" ref="E16:G18" si="3">E15-B16</f>
+        <v>0.1428571428571429</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="3"/>
+        <v>0.15436241610738261</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="3"/>
+        <v>0.12621359223300971</v>
+      </c>
       <c r="J16">
         <f>B15</f>
         <v>0.33730158730158732</v>
@@ -648,12 +716,24 @@
         <f t="shared" si="2"/>
         <v>0.10679611650485436</v>
       </c>
+      <c r="E17">
+        <f t="shared" si="3"/>
+        <v>2.7777777777777832E-2</v>
+      </c>
+      <c r="F17">
+        <f t="shared" si="3"/>
+        <v>3.3557046979865821E-2</v>
+      </c>
+      <c r="G17">
+        <f t="shared" si="3"/>
+        <v>1.9417475728155345E-2</v>
+      </c>
       <c r="J17">
         <f>B16</f>
         <v>6.7460317460317457E-2</v>
       </c>
       <c r="K17">
-        <f t="shared" ref="K17:K19" si="3">K16-J17</f>
+        <f t="shared" ref="K17:K19" si="4">K16-J17</f>
         <v>0.1428571428571429</v>
       </c>
       <c r="L17">
@@ -678,12 +758,24 @@
         <f t="shared" si="2"/>
         <v>1.9417475728155338E-2</v>
       </c>
+      <c r="E18">
+        <f t="shared" si="3"/>
+        <v>5.5511151231257827E-17</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G18">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="J18">
         <f>B17</f>
         <v>0.11507936507936507</v>
       </c>
       <c r="K18">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.7777777777777832E-2</v>
       </c>
       <c r="L18">
@@ -697,8 +789,22 @@
         <v>2.7777777777777776E-2</v>
       </c>
       <c r="K19">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.5511151231257827E-17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="B20">
+        <f>SUM(B14:B18)</f>
+        <v>1</v>
+      </c>
+      <c r="C20">
+        <f>SUM(C14:C18)</f>
+        <v>1</v>
+      </c>
+      <c r="D20">
+        <f>SUM(D14:D18)</f>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>